<commit_message>
latest update updated the template and functions of LOTS
</commit_message>
<xml_diff>
--- a/res/template/Load_Plan_Template.xlsx
+++ b/res/template/Load_Plan_Template.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\5CG6105SVT\Desktop\LoadPlan_Automation\res\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5164B03-6D9F-4D99-9B5B-4C3BFCD3B86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7087BDC7-1090-4335-88F6-2805CF3DC413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{E31B4C9E-2B2E-4045-962C-05F8A6B83FCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -283,6 +283,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -296,12 +297,14 @@
       <sz val="8"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -444,6 +447,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -476,9 +482,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -900,83 +903,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="32" t="e" vm="1">
+      <c r="B1" s="33" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="33" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="35" t="s">
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
     </row>
     <row r="2" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
     </row>
     <row r="3" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="34" t="s">
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="36"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
     </row>
     <row r="5" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -990,145 +993,145 @@
       <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
       <c r="E6" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
       <c r="K6" s="9"/>
       <c r="L6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="31" t="s">
+      <c r="M6" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
     </row>
     <row r="7" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
     </row>
     <row r="10" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="29" t="s">
+      <c r="F10" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29" t="s">
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="M10" s="29" t="s">
+      <c r="M10" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="N10" s="29" t="s">
+      <c r="N10" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="O10" s="29" t="s">
+      <c r="O10" s="30" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="27"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
     </row>
     <row r="12" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="27"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
       <c r="G12" s="6" t="s">
         <v>17</v>
       </c>
@@ -1144,17 +1147,17 @@
       <c r="K12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="38"/>
+      <c r="E13" s="27"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -1546,10 +1549,10 @@
       </c>
       <c r="C37" s="12"/>
       <c r="D37" s="1"/>
-      <c r="E37" s="36" t="s">
+      <c r="E37" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="F37" s="37"/>
+      <c r="F37" s="38"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="16"/>

</xml_diff>